<commit_message>
Arreglado bug que no permitia general excel en ingreso de inventarios
</commit_message>
<xml_diff>
--- a/reportes/ingresos/Reporte 19-07-2017.xlsx
+++ b/reportes/ingresos/Reporte 19-07-2017.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Fecha de Compra</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Nuevo</t>
-  </si>
-  <si>
-    <t>17-07-2017</t>
   </si>
 </sst>
 </file>
@@ -401,7 +398,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,107 +484,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1221</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3">
-        <v>12124</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1221</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4">
-        <v>4242</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>22222</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>1212</v>
-      </c>
-      <c r="H5">
-        <v>212</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>